<commit_message>
Test Design Integration test
</commit_message>
<xml_diff>
--- a/docs/tests/TestDesign/03_API_Test_Design_Template.xlsx
+++ b/docs/tests/TestDesign/03_API_Test_Design_Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2371C1496C8AE60E/Tài liệu/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KiemThuPhanMem_Web\fullstack-vitejs-books\docs\tests\TestDesign\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="362" documentId="8_{7150459B-AC7A-48F8-A17A-2B8ADC81D2D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF40D0D0-25B8-4881-8BA6-47F361DFF575}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7D3812E-A7ED-41F7-B3F1-8EDB37978F62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{BAB9F688-AB70-402F-97B8-951CC23A1191}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BAB9F688-AB70-402F-97B8-951CC23A1191}"/>
   </bookViews>
   <sheets>
     <sheet name="AccessControl" sheetId="6" r:id="rId1"/>
@@ -1393,18 +1393,18 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1716,8 +1716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59E978E5-B5C7-4118-B506-AF816C63F822}">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1734,19 +1734,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.8">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
     </row>
     <row r="2" spans="1:9" ht="19.8">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1766,38 +1766,38 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="17.399999999999999">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-    </row>
-    <row r="8" spans="1:9" s="3" customFormat="1">
-      <c r="A8" s="3" t="s">
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+    </row>
+    <row r="8" spans="1:9" s="1" customFormat="1">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1889,41 +1889,41 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="17.399999999999999">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="3" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="3" customFormat="1">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:9" s="1" customFormat="1">
+      <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="H15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I15" s="3" t="s">
+      <c r="I15" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1986,36 +1986,36 @@
       </c>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="3" customFormat="1">
-      <c r="A20" s="3" t="s">
+    <row r="20" spans="1:9" s="1" customFormat="1">
+      <c r="A20" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="G20" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="H20" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I20" s="3" t="s">
+      <c r="I20" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2078,36 +2078,36 @@
       </c>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="1:9" s="3" customFormat="1">
-      <c r="A25" s="3" t="s">
+    <row r="25" spans="1:9" s="1" customFormat="1">
+      <c r="A25" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E25" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F25" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="G25" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H25" s="3" t="s">
+      <c r="H25" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I25" s="3" t="s">
+      <c r="I25" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2141,36 +2141,36 @@
       </c>
     </row>
     <row r="28" spans="1:9">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="1:9" s="3" customFormat="1">
-      <c r="A29" s="3" t="s">
+    <row r="29" spans="1:9" s="1" customFormat="1">
+      <c r="A29" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D29" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E29" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="F29" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G29" s="3" t="s">
+      <c r="G29" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H29" s="3" t="s">
+      <c r="H29" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I29" s="3" t="s">
+      <c r="I29" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2233,36 +2233,36 @@
       </c>
     </row>
     <row r="33" spans="1:9">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="1:9" s="3" customFormat="1">
-      <c r="A34" s="3" t="s">
+    <row r="34" spans="1:9" s="1" customFormat="1">
+      <c r="A34" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="E34" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F34" s="3" t="s">
+      <c r="F34" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G34" s="3" t="s">
+      <c r="G34" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H34" s="3" t="s">
+      <c r="H34" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I34" s="3" t="s">
+      <c r="I34" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2325,36 +2325,36 @@
       </c>
     </row>
     <row r="38" spans="1:9">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="39" spans="1:9" s="3" customFormat="1">
-      <c r="A39" s="3" t="s">
+    <row r="39" spans="1:9" s="1" customFormat="1">
+      <c r="A39" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C39" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="D39" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E39" s="3" t="s">
+      <c r="E39" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F39" s="3" t="s">
+      <c r="F39" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G39" s="3" t="s">
+      <c r="G39" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H39" s="3" t="s">
+      <c r="H39" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I39" s="3" t="s">
+      <c r="I39" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2417,19 +2417,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.8">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
     </row>
     <row r="2" spans="1:9" ht="19.8">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2449,36 +2449,36 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="17.399999999999999">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="3" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="3" customFormat="1">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:9" s="1" customFormat="1">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2541,36 +2541,36 @@
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="3" customFormat="1">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:9" s="1" customFormat="1">
+      <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="H13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I13" s="3" t="s">
+      <c r="I13" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2604,36 +2604,36 @@
       </c>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="3" customFormat="1">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:9" s="1" customFormat="1">
+      <c r="A17" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G17" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="H17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I17" s="3" t="s">
+      <c r="I17" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2667,36 +2667,36 @@
       </c>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="3" customFormat="1">
-      <c r="A21" s="3" t="s">
+    <row r="21" spans="1:9" s="1" customFormat="1">
+      <c r="A21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="G21" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="H21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I21" s="3" t="s">
+      <c r="I21" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2741,7 +2741,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8CEAD67-A364-469E-A1AE-38945F552139}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
@@ -2756,19 +2756,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.8">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
     </row>
     <row r="2" spans="1:9" ht="19.8">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2788,36 +2788,36 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="17.399999999999999">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="3" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="3" customFormat="1">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:9" s="1" customFormat="1">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2851,36 +2851,36 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="17.399999999999999">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="3" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="3" customFormat="1">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:9" s="1" customFormat="1">
+      <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="I12" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2914,36 +2914,36 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="17.399999999999999">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="3" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="3" customFormat="1">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:9" s="1" customFormat="1">
+      <c r="A16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="H16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I16" s="3" t="s">
+      <c r="I16" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2977,36 +2977,36 @@
       </c>
     </row>
     <row r="19" spans="1:9" ht="17.399999999999999">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="3" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="3" customFormat="1">
-      <c r="A20" s="3" t="s">
+    <row r="20" spans="1:9" s="1" customFormat="1">
+      <c r="A20" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="G20" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="H20" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I20" s="3" t="s">
+      <c r="I20" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3066,19 +3066,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.8">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
     </row>
     <row r="2" spans="1:9" ht="19.8">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -3098,36 +3098,36 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="17.399999999999999">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="3" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="3" customFormat="1">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:9" s="1" customFormat="1">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3161,36 +3161,36 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="17.399999999999999">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="3" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="3" customFormat="1">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:9" s="1" customFormat="1">
+      <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="I12" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3224,36 +3224,36 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="17.399999999999999">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="3" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="3" customFormat="1">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:9" s="1" customFormat="1">
+      <c r="A16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="H16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I16" s="3" t="s">
+      <c r="I16" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3287,36 +3287,36 @@
       </c>
     </row>
     <row r="19" spans="1:9" ht="17.399999999999999">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="3" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="3" customFormat="1">
-      <c r="A20" s="3" t="s">
+    <row r="20" spans="1:9" s="1" customFormat="1">
+      <c r="A20" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="G20" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="H20" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I20" s="3" t="s">
+      <c r="I20" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3350,36 +3350,36 @@
       </c>
     </row>
     <row r="23" spans="1:9" ht="17.399999999999999">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="3" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="24" spans="1:9" s="3" customFormat="1">
-      <c r="A24" s="3" t="s">
+    <row r="24" spans="1:9" s="1" customFormat="1">
+      <c r="A24" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E24" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F24" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G24" s="3" t="s">
+      <c r="G24" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H24" s="3" t="s">
+      <c r="H24" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I24" s="3" t="s">
+      <c r="I24" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3413,36 +3413,36 @@
       </c>
     </row>
     <row r="27" spans="1:9" ht="17.399999999999999">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="3" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="28" spans="1:9" s="3" customFormat="1">
-      <c r="A28" s="3" t="s">
+    <row r="28" spans="1:9" s="1" customFormat="1">
+      <c r="A28" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="E28" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="F28" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G28" s="3" t="s">
+      <c r="G28" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H28" s="3" t="s">
+      <c r="H28" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I28" s="3" t="s">
+      <c r="I28" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3476,36 +3476,36 @@
       </c>
     </row>
     <row r="31" spans="1:9" ht="17.399999999999999">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="3" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="32" spans="1:9" s="3" customFormat="1">
-      <c r="A32" s="3" t="s">
+    <row r="32" spans="1:9" s="1" customFormat="1">
+      <c r="A32" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="E32" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="F32" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G32" s="3" t="s">
+      <c r="G32" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H32" s="3" t="s">
+      <c r="H32" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I32" s="3" t="s">
+      <c r="I32" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3565,19 +3565,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.8">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
     </row>
     <row r="2" spans="1:9" ht="19.8">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -3597,36 +3597,36 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="17.399999999999999">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="3" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="3" customFormat="1">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:9" s="1" customFormat="1">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3660,36 +3660,36 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="17.399999999999999">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="3" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="3" customFormat="1">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:9" s="1" customFormat="1">
+      <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="I12" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3723,36 +3723,36 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="17.399999999999999">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="3" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="3" customFormat="1">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:9" s="1" customFormat="1">
+      <c r="A16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="H16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I16" s="3" t="s">
+      <c r="I16" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3786,36 +3786,36 @@
       </c>
     </row>
     <row r="20" spans="1:9" ht="17.399999999999999">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="3" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="3" customFormat="1">
-      <c r="A21" s="3" t="s">
+    <row r="21" spans="1:9" s="1" customFormat="1">
+      <c r="A21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="G21" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="H21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I21" s="3" t="s">
+      <c r="I21" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3849,36 +3849,36 @@
       </c>
     </row>
     <row r="24" spans="1:9" ht="17.399999999999999">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="25" spans="1:9" s="3" customFormat="1">
-      <c r="A25" s="3" t="s">
+    <row r="25" spans="1:9" s="1" customFormat="1">
+      <c r="A25" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E25" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F25" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="G25" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H25" s="3" t="s">
+      <c r="H25" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I25" s="3" t="s">
+      <c r="I25" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3912,36 +3912,36 @@
       </c>
     </row>
     <row r="28" spans="1:9" ht="17.399999999999999">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="3" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="29" spans="1:9" s="3" customFormat="1">
-      <c r="A29" s="3" t="s">
+    <row r="29" spans="1:9" s="1" customFormat="1">
+      <c r="A29" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D29" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E29" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="F29" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G29" s="3" t="s">
+      <c r="G29" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H29" s="3" t="s">
+      <c r="H29" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I29" s="3" t="s">
+      <c r="I29" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4001,19 +4001,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.8">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
     </row>
     <row r="2" spans="1:9" ht="19.8">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -4043,41 +4043,41 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="17.399999999999999">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="3" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="1" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="3" customFormat="1">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:9" s="1" customFormat="1">
+      <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="H11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="I11" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4111,36 +4111,36 @@
       </c>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="1" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="3" customFormat="1">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:9" s="1" customFormat="1">
+      <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="H15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I15" s="3" t="s">
+      <c r="I15" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4174,36 +4174,36 @@
       </c>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="1" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="3" customFormat="1">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:9" s="1" customFormat="1">
+      <c r="A19" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="G19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="H19" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I19" s="3" t="s">
+      <c r="I19" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4237,36 +4237,36 @@
       </c>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="1" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="23" spans="1:9" s="3" customFormat="1">
-      <c r="A23" s="3" t="s">
+    <row r="23" spans="1:9" s="1" customFormat="1">
+      <c r="A23" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E23" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="G23" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="H23" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I23" s="3" t="s">
+      <c r="I23" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4300,36 +4300,36 @@
       </c>
     </row>
     <row r="26" spans="1:9">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="1" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="27" spans="1:9" s="3" customFormat="1">
-      <c r="A27" s="3" t="s">
+    <row r="27" spans="1:9" s="1" customFormat="1">
+      <c r="A27" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="E27" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="F27" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G27" s="3" t="s">
+      <c r="G27" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H27" s="3" t="s">
+      <c r="H27" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I27" s="3" t="s">
+      <c r="I27" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4363,36 +4363,36 @@
       </c>
     </row>
     <row r="30" spans="1:9">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="1" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="31" spans="1:9" s="3" customFormat="1">
-      <c r="A31" s="3" t="s">
+    <row r="31" spans="1:9" s="1" customFormat="1">
+      <c r="A31" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E31" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="F31" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G31" s="3" t="s">
+      <c r="G31" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H31" s="3" t="s">
+      <c r="H31" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I31" s="3" t="s">
+      <c r="I31" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4426,41 +4426,41 @@
       </c>
     </row>
     <row r="34" spans="1:9" ht="17.399999999999999">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="3" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="35" spans="1:9">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="1" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="36" spans="1:9" s="3" customFormat="1">
-      <c r="A36" s="3" t="s">
+    <row r="36" spans="1:9" s="1" customFormat="1">
+      <c r="A36" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D36" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E36" s="3" t="s">
+      <c r="E36" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F36" s="3" t="s">
+      <c r="F36" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G36" s="3" t="s">
+      <c r="G36" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H36" s="3" t="s">
+      <c r="H36" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I36" s="3" t="s">
+      <c r="I36" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4494,36 +4494,36 @@
       </c>
     </row>
     <row r="39" spans="1:9">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="1" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="40" spans="1:9" s="3" customFormat="1">
-      <c r="A40" s="3" t="s">
+    <row r="40" spans="1:9" s="1" customFormat="1">
+      <c r="A40" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C40" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D40" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E40" s="3" t="s">
+      <c r="E40" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F40" s="3" t="s">
+      <c r="F40" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G40" s="3" t="s">
+      <c r="G40" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H40" s="3" t="s">
+      <c r="H40" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I40" s="3" t="s">
+      <c r="I40" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4557,36 +4557,36 @@
       </c>
     </row>
     <row r="43" spans="1:9">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="1" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="44" spans="1:9" s="3" customFormat="1">
-      <c r="A44" s="3" t="s">
+    <row r="44" spans="1:9" s="1" customFormat="1">
+      <c r="A44" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C44" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="D44" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E44" s="3" t="s">
+      <c r="E44" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F44" s="3" t="s">
+      <c r="F44" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G44" s="3" t="s">
+      <c r="G44" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H44" s="3" t="s">
+      <c r="H44" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I44" s="3" t="s">
+      <c r="I44" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4620,36 +4620,36 @@
       </c>
     </row>
     <row r="47" spans="1:9">
-      <c r="A47" s="3" t="s">
+      <c r="A47" s="1" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="48" spans="1:9" s="3" customFormat="1">
-      <c r="A48" s="3" t="s">
+    <row r="48" spans="1:9" s="1" customFormat="1">
+      <c r="A48" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C48" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="D48" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E48" s="3" t="s">
+      <c r="E48" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F48" s="3" t="s">
+      <c r="F48" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G48" s="3" t="s">
+      <c r="G48" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H48" s="3" t="s">
+      <c r="H48" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I48" s="3" t="s">
+      <c r="I48" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4683,36 +4683,36 @@
       </c>
     </row>
     <row r="51" spans="1:9">
-      <c r="A51" s="3" t="s">
+      <c r="A51" s="1" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="52" spans="1:9" s="3" customFormat="1">
-      <c r="A52" s="3" t="s">
+    <row r="52" spans="1:9" s="1" customFormat="1">
+      <c r="A52" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B52" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="C52" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D52" s="3" t="s">
+      <c r="D52" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E52" s="3" t="s">
+      <c r="E52" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F52" s="3" t="s">
+      <c r="F52" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G52" s="3" t="s">
+      <c r="G52" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H52" s="3" t="s">
+      <c r="H52" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I52" s="3" t="s">
+      <c r="I52" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4746,36 +4746,36 @@
       </c>
     </row>
     <row r="55" spans="1:9">
-      <c r="A55" s="3" t="s">
+      <c r="A55" s="1" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="56" spans="1:9" s="3" customFormat="1">
-      <c r="A56" s="3" t="s">
+    <row r="56" spans="1:9" s="1" customFormat="1">
+      <c r="A56" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B56" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C56" s="3" t="s">
+      <c r="C56" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D56" s="3" t="s">
+      <c r="D56" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E56" s="3" t="s">
+      <c r="E56" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F56" s="3" t="s">
+      <c r="F56" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G56" s="3" t="s">
+      <c r="G56" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H56" s="3" t="s">
+      <c r="H56" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I56" s="3" t="s">
+      <c r="I56" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4809,36 +4809,36 @@
       </c>
     </row>
     <row r="59" spans="1:9">
-      <c r="A59" s="3" t="s">
+      <c r="A59" s="1" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="60" spans="1:9" s="3" customFormat="1">
-      <c r="A60" s="3" t="s">
+    <row r="60" spans="1:9" s="1" customFormat="1">
+      <c r="A60" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="B60" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C60" s="3" t="s">
+      <c r="C60" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D60" s="3" t="s">
+      <c r="D60" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E60" s="3" t="s">
+      <c r="E60" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F60" s="3" t="s">
+      <c r="F60" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G60" s="3" t="s">
+      <c r="G60" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H60" s="3" t="s">
+      <c r="H60" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I60" s="3" t="s">
+      <c r="I60" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4872,36 +4872,36 @@
       </c>
     </row>
     <row r="63" spans="1:9">
-      <c r="A63" s="3" t="s">
+      <c r="A63" s="1" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="64" spans="1:9" s="3" customFormat="1">
-      <c r="A64" s="3" t="s">
+    <row r="64" spans="1:9" s="1" customFormat="1">
+      <c r="A64" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B64" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="C64" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D64" s="3" t="s">
+      <c r="D64" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E64" s="3" t="s">
+      <c r="E64" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F64" s="3" t="s">
+      <c r="F64" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G64" s="3" t="s">
+      <c r="G64" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H64" s="3" t="s">
+      <c r="H64" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I64" s="3" t="s">
+      <c r="I64" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4935,36 +4935,36 @@
       </c>
     </row>
     <row r="67" spans="1:10">
-      <c r="A67" s="3" t="s">
+      <c r="A67" s="1" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="68" spans="1:10" s="3" customFormat="1">
-      <c r="A68" s="3" t="s">
+    <row r="68" spans="1:10" s="1" customFormat="1">
+      <c r="A68" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="B68" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C68" s="3" t="s">
+      <c r="C68" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D68" s="3" t="s">
+      <c r="D68" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E68" s="3" t="s">
+      <c r="E68" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F68" s="3" t="s">
+      <c r="F68" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G68" s="3" t="s">
+      <c r="G68" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H68" s="3" t="s">
+      <c r="H68" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I68" s="3" t="s">
+      <c r="I68" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5001,36 +5001,36 @@
       </c>
     </row>
     <row r="71" spans="1:10">
-      <c r="A71" s="3" t="s">
+      <c r="A71" s="1" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="72" spans="1:10" s="3" customFormat="1">
-      <c r="A72" s="3" t="s">
+    <row r="72" spans="1:10" s="1" customFormat="1">
+      <c r="A72" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B72" s="3" t="s">
+      <c r="B72" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C72" s="3" t="s">
+      <c r="C72" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D72" s="3" t="s">
+      <c r="D72" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E72" s="3" t="s">
+      <c r="E72" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F72" s="3" t="s">
+      <c r="F72" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G72" s="3" t="s">
+      <c r="G72" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H72" s="3" t="s">
+      <c r="H72" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I72" s="3" t="s">
+      <c r="I72" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5064,41 +5064,41 @@
       </c>
     </row>
     <row r="75" spans="1:10" ht="17.399999999999999">
-      <c r="A75" s="6" t="s">
+      <c r="A75" s="3" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="76" spans="1:10">
-      <c r="A76" s="3" t="s">
+      <c r="A76" s="1" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="77" spans="1:10" s="3" customFormat="1">
-      <c r="A77" s="3" t="s">
+    <row r="77" spans="1:10" s="1" customFormat="1">
+      <c r="A77" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="B77" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C77" s="3" t="s">
+      <c r="C77" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D77" s="3" t="s">
+      <c r="D77" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E77" s="3" t="s">
+      <c r="E77" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F77" s="3" t="s">
+      <c r="F77" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G77" s="3" t="s">
+      <c r="G77" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H77" s="3" t="s">
+      <c r="H77" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I77" s="3" t="s">
+      <c r="I77" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5132,36 +5132,36 @@
       </c>
     </row>
     <row r="80" spans="1:10">
-      <c r="A80" s="3" t="s">
+      <c r="A80" s="1" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="81" spans="1:9" s="3" customFormat="1">
-      <c r="A81" s="3" t="s">
+    <row r="81" spans="1:9" s="1" customFormat="1">
+      <c r="A81" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B81" s="3" t="s">
+      <c r="B81" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C81" s="3" t="s">
+      <c r="C81" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D81" s="3" t="s">
+      <c r="D81" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E81" s="3" t="s">
+      <c r="E81" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F81" s="3" t="s">
+      <c r="F81" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G81" s="3" t="s">
+      <c r="G81" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H81" s="3" t="s">
+      <c r="H81" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I81" s="3" t="s">
+      <c r="I81" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5195,36 +5195,36 @@
       </c>
     </row>
     <row r="84" spans="1:9">
-      <c r="A84" s="3" t="s">
+      <c r="A84" s="1" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="85" spans="1:9" s="3" customFormat="1">
-      <c r="A85" s="3" t="s">
+    <row r="85" spans="1:9" s="1" customFormat="1">
+      <c r="A85" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B85" s="3" t="s">
+      <c r="B85" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C85" s="3" t="s">
+      <c r="C85" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D85" s="3" t="s">
+      <c r="D85" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E85" s="3" t="s">
+      <c r="E85" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F85" s="3" t="s">
+      <c r="F85" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G85" s="3" t="s">
+      <c r="G85" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H85" s="3" t="s">
+      <c r="H85" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I85" s="3" t="s">
+      <c r="I85" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5258,36 +5258,36 @@
       </c>
     </row>
     <row r="88" spans="1:9">
-      <c r="A88" s="3" t="s">
+      <c r="A88" s="1" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="89" spans="1:9" s="3" customFormat="1">
-      <c r="A89" s="3" t="s">
+    <row r="89" spans="1:9" s="1" customFormat="1">
+      <c r="A89" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B89" s="3" t="s">
+      <c r="B89" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C89" s="3" t="s">
+      <c r="C89" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D89" s="3" t="s">
+      <c r="D89" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E89" s="3" t="s">
+      <c r="E89" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F89" s="3" t="s">
+      <c r="F89" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G89" s="3" t="s">
+      <c r="G89" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H89" s="3" t="s">
+      <c r="H89" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I89" s="3" t="s">
+      <c r="I89" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5321,36 +5321,36 @@
       </c>
     </row>
     <row r="92" spans="1:9">
-      <c r="A92" s="3" t="s">
+      <c r="A92" s="1" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="93" spans="1:9" s="3" customFormat="1">
-      <c r="A93" s="3" t="s">
+    <row r="93" spans="1:9" s="1" customFormat="1">
+      <c r="A93" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B93" s="3" t="s">
+      <c r="B93" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C93" s="3" t="s">
+      <c r="C93" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D93" s="3" t="s">
+      <c r="D93" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E93" s="3" t="s">
+      <c r="E93" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F93" s="3" t="s">
+      <c r="F93" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G93" s="3" t="s">
+      <c r="G93" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H93" s="3" t="s">
+      <c r="H93" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I93" s="3" t="s">
+      <c r="I93" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5384,36 +5384,36 @@
       </c>
     </row>
     <row r="96" spans="1:9">
-      <c r="A96" s="3" t="s">
+      <c r="A96" s="1" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="97" spans="1:9" s="3" customFormat="1">
-      <c r="A97" s="3" t="s">
+    <row r="97" spans="1:9" s="1" customFormat="1">
+      <c r="A97" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B97" s="3" t="s">
+      <c r="B97" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C97" s="3" t="s">
+      <c r="C97" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D97" s="3" t="s">
+      <c r="D97" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E97" s="3" t="s">
+      <c r="E97" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F97" s="3" t="s">
+      <c r="F97" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G97" s="3" t="s">
+      <c r="G97" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H97" s="3" t="s">
+      <c r="H97" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I97" s="3" t="s">
+      <c r="I97" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5447,36 +5447,36 @@
       </c>
     </row>
     <row r="100" spans="1:9">
-      <c r="A100" s="3" t="s">
+      <c r="A100" s="1" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="101" spans="1:9" s="3" customFormat="1">
-      <c r="A101" s="3" t="s">
+    <row r="101" spans="1:9" s="1" customFormat="1">
+      <c r="A101" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B101" s="3" t="s">
+      <c r="B101" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C101" s="3" t="s">
+      <c r="C101" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D101" s="3" t="s">
+      <c r="D101" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E101" s="3" t="s">
+      <c r="E101" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F101" s="3" t="s">
+      <c r="F101" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G101" s="3" t="s">
+      <c r="G101" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H101" s="3" t="s">
+      <c r="H101" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I101" s="3" t="s">
+      <c r="I101" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5510,41 +5510,41 @@
       </c>
     </row>
     <row r="104" spans="1:9" ht="17.399999999999999">
-      <c r="A104" s="6" t="s">
+      <c r="A104" s="3" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="105" spans="1:9">
-      <c r="A105" s="3" t="s">
+      <c r="A105" s="1" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="106" spans="1:9" s="3" customFormat="1">
-      <c r="A106" s="3" t="s">
+    <row r="106" spans="1:9" s="1" customFormat="1">
+      <c r="A106" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B106" s="3" t="s">
+      <c r="B106" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C106" s="3" t="s">
+      <c r="C106" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D106" s="3" t="s">
+      <c r="D106" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E106" s="3" t="s">
+      <c r="E106" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F106" s="3" t="s">
+      <c r="F106" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G106" s="3" t="s">
+      <c r="G106" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H106" s="3" t="s">
+      <c r="H106" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I106" s="3" t="s">
+      <c r="I106" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5578,36 +5578,36 @@
       </c>
     </row>
     <row r="109" spans="1:9">
-      <c r="A109" s="3" t="s">
+      <c r="A109" s="1" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="110" spans="1:9" s="3" customFormat="1">
-      <c r="A110" s="3" t="s">
+    <row r="110" spans="1:9" s="1" customFormat="1">
+      <c r="A110" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B110" s="3" t="s">
+      <c r="B110" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C110" s="3" t="s">
+      <c r="C110" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D110" s="3" t="s">
+      <c r="D110" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E110" s="3" t="s">
+      <c r="E110" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F110" s="3" t="s">
+      <c r="F110" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G110" s="3" t="s">
+      <c r="G110" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H110" s="3" t="s">
+      <c r="H110" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I110" s="3" t="s">
+      <c r="I110" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5641,24 +5641,24 @@
       </c>
     </row>
     <row r="113" spans="1:5">
-      <c r="A113" s="3" t="s">
+      <c r="A113" s="1" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="114" spans="1:5" s="3" customFormat="1">
-      <c r="A114" s="3" t="s">
+    <row r="114" spans="1:5" s="1" customFormat="1">
+      <c r="A114" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B114" s="3" t="s">
+      <c r="B114" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C114" s="3" t="s">
+      <c r="C114" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D114" s="3" t="s">
+      <c r="D114" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E114" s="3" t="s">
+      <c r="E114" s="1" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>